<commit_message>
Update on the code as of June 2025
</commit_message>
<xml_diff>
--- a/Excel/ARP_LSZT_012025.xlsx
+++ b/Excel/ARP_LSZT_012025.xlsx
@@ -1015,7 +1015,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O63"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="B3" s="27" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="C3" s="27" t="n">
@@ -1147,7 +1147,7 @@
       </c>
       <c r="E3" s="27" t="inlineStr">
         <is>
-          <t>1407</t>
+          <t>1050</t>
         </is>
       </c>
       <c r="F3" s="27" t="inlineStr">
@@ -1165,12 +1165,12 @@
       </c>
       <c r="I3" s="27" t="inlineStr">
         <is>
-          <t>HBKPJ</t>
+          <t>HBYVC</t>
         </is>
       </c>
       <c r="J3" s="27" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>24</t>
         </is>
       </c>
       <c r="K3" s="27" t="n">
@@ -1212,12 +1212,12 @@
       </c>
       <c r="E4" s="27" t="inlineStr">
         <is>
-          <t>1050</t>
+          <t>1249</t>
         </is>
       </c>
       <c r="F4" s="27" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G4" s="27" t="n">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="N4" s="27" t="inlineStr">
         <is>
-          <t>LSZT</t>
+          <t>LSZZ</t>
         </is>
       </c>
       <c r="O4" s="27" t="inlineStr">
@@ -1277,12 +1277,12 @@
       </c>
       <c r="E5" s="27" t="inlineStr">
         <is>
-          <t>1053</t>
+          <t>1303</t>
         </is>
       </c>
       <c r="F5" s="27" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G5" s="27" t="n">
@@ -1295,12 +1295,12 @@
       </c>
       <c r="I5" s="27" t="inlineStr">
         <is>
-          <t>HBYVC</t>
+          <t>HBKLR</t>
         </is>
       </c>
       <c r="J5" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>06</t>
         </is>
       </c>
       <c r="K5" s="27" t="n">
@@ -1314,7 +1314,7 @@
       </c>
       <c r="N5" s="27" t="inlineStr">
         <is>
-          <t>LSZT</t>
+          <t>LSZZ</t>
         </is>
       </c>
       <c r="O5" s="27" t="inlineStr">
@@ -1342,7 +1342,7 @@
       </c>
       <c r="E6" s="27" t="inlineStr">
         <is>
-          <t>1242</t>
+          <t>1400</t>
         </is>
       </c>
       <c r="F6" s="27" t="inlineStr">
@@ -1360,7 +1360,7 @@
       </c>
       <c r="I6" s="27" t="inlineStr">
         <is>
-          <t>HBYVC</t>
+          <t>HBKLA</t>
         </is>
       </c>
       <c r="J6" s="27" t="inlineStr">
@@ -1384,7 +1384,7 @@
       </c>
       <c r="O6" s="27" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>SW</t>
         </is>
       </c>
     </row>
@@ -1407,12 +1407,12 @@
       </c>
       <c r="E7" s="27" t="inlineStr">
         <is>
-          <t>1249</t>
+          <t>1400</t>
         </is>
       </c>
       <c r="F7" s="27" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>V</t>
         </is>
       </c>
       <c r="G7" s="27" t="n">
@@ -1425,7 +1425,7 @@
       </c>
       <c r="I7" s="27" t="inlineStr">
         <is>
-          <t>HBYVC</t>
+          <t>HBKLA</t>
         </is>
       </c>
       <c r="J7" s="27" t="inlineStr">
@@ -1434,7 +1434,7 @@
         </is>
       </c>
       <c r="K7" s="27" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L7" s="27" t="n">
         <v>0</v>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="O7" s="27" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1472,12 +1472,12 @@
       </c>
       <c r="E8" s="27" t="inlineStr">
         <is>
-          <t>1303</t>
+          <t>1430</t>
         </is>
       </c>
       <c r="F8" s="27" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G8" s="27" t="n">
@@ -1495,7 +1495,7 @@
       </c>
       <c r="J8" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>06</t>
         </is>
       </c>
       <c r="K8" s="27" t="n">
@@ -1509,7 +1509,7 @@
       </c>
       <c r="N8" s="27" t="inlineStr">
         <is>
-          <t>LSZT</t>
+          <t>LSZZ</t>
         </is>
       </c>
       <c r="O8" s="27" t="inlineStr">
@@ -1537,7 +1537,7 @@
       </c>
       <c r="E9" s="27" t="inlineStr">
         <is>
-          <t>1307</t>
+          <t>1444</t>
         </is>
       </c>
       <c r="F9" s="27" t="inlineStr">
@@ -1555,12 +1555,12 @@
       </c>
       <c r="I9" s="27" t="inlineStr">
         <is>
-          <t>HBKLR</t>
+          <t>HBKLA</t>
         </is>
       </c>
       <c r="J9" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>06</t>
         </is>
       </c>
       <c r="K9" s="27" t="n">
@@ -1579,7 +1579,7 @@
       </c>
       <c r="O9" s="27" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="B10" s="27" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="C10" s="27" t="n">
@@ -1602,7 +1602,7 @@
       </c>
       <c r="E10" s="27" t="inlineStr">
         <is>
-          <t>1400</t>
+          <t>1418</t>
         </is>
       </c>
       <c r="F10" s="27" t="inlineStr">
@@ -1620,7 +1620,7 @@
       </c>
       <c r="I10" s="27" t="inlineStr">
         <is>
-          <t>HBKLA</t>
+          <t>HBKFW</t>
         </is>
       </c>
       <c r="J10" s="27" t="inlineStr">
@@ -1644,7 +1644,7 @@
       </c>
       <c r="O10" s="27" t="inlineStr">
         <is>
-          <t>SW</t>
+          <t>SO</t>
         </is>
       </c>
     </row>
@@ -1656,7 +1656,7 @@
       </c>
       <c r="B11" s="27" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="C11" s="27" t="n">
@@ -1667,12 +1667,12 @@
       </c>
       <c r="E11" s="27" t="inlineStr">
         <is>
-          <t>1400</t>
+          <t>1528</t>
         </is>
       </c>
       <c r="F11" s="27" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G11" s="27" t="n">
@@ -1685,16 +1685,16 @@
       </c>
       <c r="I11" s="27" t="inlineStr">
         <is>
-          <t>HBKLA</t>
+          <t>HBKFW</t>
         </is>
       </c>
       <c r="J11" s="27" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>24</t>
         </is>
       </c>
       <c r="K11" s="27" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="L11" s="27" t="n">
         <v>0</v>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="O11" s="27" t="inlineStr">
         <is>
-          <t>SW</t>
+          <t>SO</t>
         </is>
       </c>
     </row>
@@ -1721,7 +1721,7 @@
       </c>
       <c r="B12" s="27" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>18</t>
         </is>
       </c>
       <c r="C12" s="27" t="n">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="E12" s="27" t="inlineStr">
         <is>
-          <t>1425</t>
+          <t>1313</t>
         </is>
       </c>
       <c r="F12" s="27" t="inlineStr">
@@ -1750,7 +1750,7 @@
       </c>
       <c r="I12" s="27" t="inlineStr">
         <is>
-          <t>HBKLR</t>
+          <t>HBKLA</t>
         </is>
       </c>
       <c r="J12" s="27" t="inlineStr">
@@ -1786,7 +1786,7 @@
       </c>
       <c r="B13" s="27" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>18</t>
         </is>
       </c>
       <c r="C13" s="27" t="n">
@@ -1797,12 +1797,12 @@
       </c>
       <c r="E13" s="27" t="inlineStr">
         <is>
-          <t>1430</t>
+          <t>1356</t>
         </is>
       </c>
       <c r="F13" s="27" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G13" s="27" t="n">
@@ -1815,12 +1815,12 @@
       </c>
       <c r="I13" s="27" t="inlineStr">
         <is>
-          <t>HBKLR</t>
+          <t>HBWYC</t>
         </is>
       </c>
       <c r="J13" s="27" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>24</t>
         </is>
       </c>
       <c r="K13" s="27" t="n">
@@ -1839,7 +1839,7 @@
       </c>
       <c r="O13" s="27" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>SW</t>
         </is>
       </c>
     </row>
@@ -1851,7 +1851,7 @@
       </c>
       <c r="B14" s="27" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>18</t>
         </is>
       </c>
       <c r="C14" s="27" t="n">
@@ -1862,7 +1862,7 @@
       </c>
       <c r="E14" s="27" t="inlineStr">
         <is>
-          <t>1444</t>
+          <t>1455</t>
         </is>
       </c>
       <c r="F14" s="27" t="inlineStr">
@@ -1885,7 +1885,7 @@
       </c>
       <c r="J14" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>06</t>
         </is>
       </c>
       <c r="K14" s="27" t="n">
@@ -1904,7 +1904,7 @@
       </c>
       <c r="O14" s="27" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SO</t>
         </is>
       </c>
     </row>
@@ -1916,7 +1916,7 @@
       </c>
       <c r="B15" s="27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>18</t>
         </is>
       </c>
       <c r="C15" s="27" t="n">
@@ -1927,12 +1927,12 @@
       </c>
       <c r="E15" s="27" t="inlineStr">
         <is>
-          <t>1418</t>
+          <t>1506</t>
         </is>
       </c>
       <c r="F15" s="27" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G15" s="27" t="n">
@@ -1945,7 +1945,7 @@
       </c>
       <c r="I15" s="27" t="inlineStr">
         <is>
-          <t>HBKFW</t>
+          <t>HBWYC</t>
         </is>
       </c>
       <c r="J15" s="27" t="inlineStr">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="B16" s="27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>24</t>
         </is>
       </c>
       <c r="C16" s="27" t="n">
@@ -1992,12 +1992,12 @@
       </c>
       <c r="E16" s="27" t="inlineStr">
         <is>
-          <t>1422</t>
+          <t>0921</t>
         </is>
       </c>
       <c r="F16" s="27" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G16" s="27" t="n">
@@ -2015,7 +2015,7 @@
       </c>
       <c r="J16" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>06</t>
         </is>
       </c>
       <c r="K16" s="27" t="n">
@@ -2029,7 +2029,7 @@
       </c>
       <c r="N16" s="27" t="inlineStr">
         <is>
-          <t>LSZT</t>
+          <t>LSZZ</t>
         </is>
       </c>
       <c r="O16" s="27" t="inlineStr">
@@ -2046,7 +2046,7 @@
       </c>
       <c r="B17" s="27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>24</t>
         </is>
       </c>
       <c r="C17" s="27" t="n">
@@ -2057,12 +2057,12 @@
       </c>
       <c r="E17" s="27" t="inlineStr">
         <is>
-          <t>1515</t>
+          <t>1008</t>
         </is>
       </c>
       <c r="F17" s="27" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G17" s="27" t="n">
@@ -2075,7 +2075,7 @@
       </c>
       <c r="I17" s="27" t="inlineStr">
         <is>
-          <t>HBSHA</t>
+          <t>HBYVC</t>
         </is>
       </c>
       <c r="J17" s="27" t="inlineStr">
@@ -2094,7 +2094,7 @@
       </c>
       <c r="N17" s="27" t="inlineStr">
         <is>
-          <t>LSZZ</t>
+          <t>LSZT</t>
         </is>
       </c>
       <c r="O17" s="27" t="inlineStr">
@@ -2111,7 +2111,7 @@
       </c>
       <c r="B18" s="27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>24</t>
         </is>
       </c>
       <c r="C18" s="27" t="n">
@@ -2122,12 +2122,12 @@
       </c>
       <c r="E18" s="27" t="inlineStr">
         <is>
-          <t>1522</t>
+          <t>1008</t>
         </is>
       </c>
       <c r="F18" s="27" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>V</t>
         </is>
       </c>
       <c r="G18" s="27" t="n">
@@ -2140,7 +2140,7 @@
       </c>
       <c r="I18" s="27" t="inlineStr">
         <is>
-          <t>HBKFW</t>
+          <t>HBYVC</t>
         </is>
       </c>
       <c r="J18" s="27" t="inlineStr">
@@ -2149,7 +2149,7 @@
         </is>
       </c>
       <c r="K18" s="27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L18" s="27" t="n">
         <v>0</v>
@@ -2164,7 +2164,7 @@
       </c>
       <c r="O18" s="27" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>SW</t>
         </is>
       </c>
     </row>
@@ -2176,7 +2176,7 @@
       </c>
       <c r="B19" s="27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>24</t>
         </is>
       </c>
       <c r="C19" s="27" t="n">
@@ -2187,12 +2187,12 @@
       </c>
       <c r="E19" s="27" t="inlineStr">
         <is>
-          <t>1528</t>
+          <t>1032</t>
         </is>
       </c>
       <c r="F19" s="27" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G19" s="27" t="n">
@@ -2205,7 +2205,7 @@
       </c>
       <c r="I19" s="27" t="inlineStr">
         <is>
-          <t>HBKFW</t>
+          <t>HBKLD</t>
         </is>
       </c>
       <c r="J19" s="27" t="inlineStr">
@@ -2241,7 +2241,7 @@
       </c>
       <c r="B20" s="27" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>24</t>
         </is>
       </c>
       <c r="C20" s="27" t="n">
@@ -2252,12 +2252,12 @@
       </c>
       <c r="E20" s="27" t="inlineStr">
         <is>
-          <t>1313</t>
+          <t>1044</t>
         </is>
       </c>
       <c r="F20" s="27" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G20" s="27" t="n">
@@ -2270,7 +2270,7 @@
       </c>
       <c r="I20" s="27" t="inlineStr">
         <is>
-          <t>HBKLA</t>
+          <t>HBYVC</t>
         </is>
       </c>
       <c r="J20" s="27" t="inlineStr">
@@ -2294,7 +2294,7 @@
       </c>
       <c r="O20" s="27" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2306,7 +2306,7 @@
       </c>
       <c r="B21" s="27" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>24</t>
         </is>
       </c>
       <c r="C21" s="27" t="n">
@@ -2317,12 +2317,12 @@
       </c>
       <c r="E21" s="27" t="inlineStr">
         <is>
-          <t>1316</t>
+          <t>1055</t>
         </is>
       </c>
       <c r="F21" s="27" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>V</t>
         </is>
       </c>
       <c r="G21" s="27" t="n">
@@ -2335,16 +2335,16 @@
       </c>
       <c r="I21" s="27" t="inlineStr">
         <is>
-          <t>HBKLA</t>
+          <t>HBKLD</t>
         </is>
       </c>
       <c r="J21" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>06</t>
         </is>
       </c>
       <c r="K21" s="27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L21" s="27" t="n">
         <v>0</v>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="O21" s="27" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>SW</t>
         </is>
       </c>
     </row>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="B22" s="27" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>24</t>
         </is>
       </c>
       <c r="C22" s="27" t="n">
@@ -2382,12 +2382,12 @@
       </c>
       <c r="E22" s="27" t="inlineStr">
         <is>
-          <t>1356</t>
+          <t>1059</t>
         </is>
       </c>
       <c r="F22" s="27" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G22" s="27" t="n">
@@ -2400,7 +2400,7 @@
       </c>
       <c r="I22" s="27" t="inlineStr">
         <is>
-          <t>HBWYC</t>
+          <t>HBKLD</t>
         </is>
       </c>
       <c r="J22" s="27" t="inlineStr">
@@ -2424,7 +2424,7 @@
       </c>
       <c r="O22" s="27" t="inlineStr">
         <is>
-          <t>SW</t>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2436,7 +2436,7 @@
       </c>
       <c r="B23" s="27" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>24</t>
         </is>
       </c>
       <c r="C23" s="27" t="n">
@@ -2447,12 +2447,12 @@
       </c>
       <c r="E23" s="27" t="inlineStr">
         <is>
-          <t>1404</t>
+          <t>1247</t>
         </is>
       </c>
       <c r="F23" s="27" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G23" s="27" t="n">
@@ -2465,7 +2465,7 @@
       </c>
       <c r="I23" s="27" t="inlineStr">
         <is>
-          <t>HBWYC</t>
+          <t>HBETG</t>
         </is>
       </c>
       <c r="J23" s="27" t="inlineStr">
@@ -2484,12 +2484,12 @@
       </c>
       <c r="N23" s="27" t="inlineStr">
         <is>
-          <t>LSZT</t>
+          <t>LSZZ</t>
         </is>
       </c>
       <c r="O23" s="27" t="inlineStr">
         <is>
-          <t>SW</t>
+          <t>SO</t>
         </is>
       </c>
     </row>
@@ -2501,7 +2501,7 @@
       </c>
       <c r="B24" s="27" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>24</t>
         </is>
       </c>
       <c r="C24" s="27" t="n">
@@ -2512,7 +2512,7 @@
       </c>
       <c r="E24" s="27" t="inlineStr">
         <is>
-          <t>1447</t>
+          <t>1258</t>
         </is>
       </c>
       <c r="F24" s="27" t="inlineStr">
@@ -2530,12 +2530,12 @@
       </c>
       <c r="I24" s="27" t="inlineStr">
         <is>
-          <t>HBWYC</t>
+          <t>HBKLD</t>
         </is>
       </c>
       <c r="J24" s="27" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>24</t>
         </is>
       </c>
       <c r="K24" s="27" t="n">
@@ -2554,7 +2554,7 @@
       </c>
       <c r="O24" s="27" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>SW</t>
         </is>
       </c>
     </row>
@@ -2566,7 +2566,7 @@
       </c>
       <c r="B25" s="27" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>24</t>
         </is>
       </c>
       <c r="C25" s="27" t="n">
@@ -2577,12 +2577,12 @@
       </c>
       <c r="E25" s="27" t="inlineStr">
         <is>
-          <t>1453</t>
+          <t>1319</t>
         </is>
       </c>
       <c r="F25" s="27" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G25" s="27" t="n">
@@ -2595,12 +2595,12 @@
       </c>
       <c r="I25" s="27" t="inlineStr">
         <is>
-          <t>HBKLA</t>
+          <t>HBKLD</t>
         </is>
       </c>
       <c r="J25" s="27" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>24</t>
         </is>
       </c>
       <c r="K25" s="27" t="n">
@@ -2619,7 +2619,7 @@
       </c>
       <c r="O25" s="27" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2631,7 +2631,7 @@
       </c>
       <c r="B26" s="27" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>24</t>
         </is>
       </c>
       <c r="C26" s="27" t="n">
@@ -2642,7 +2642,7 @@
       </c>
       <c r="E26" s="27" t="inlineStr">
         <is>
-          <t>1455</t>
+          <t>1346</t>
         </is>
       </c>
       <c r="F26" s="27" t="inlineStr">
@@ -2660,7 +2660,7 @@
       </c>
       <c r="I26" s="27" t="inlineStr">
         <is>
-          <t>HBKLA</t>
+          <t>HBETG</t>
         </is>
       </c>
       <c r="J26" s="27" t="inlineStr">
@@ -2679,12 +2679,12 @@
       </c>
       <c r="N26" s="27" t="inlineStr">
         <is>
-          <t>LSZT</t>
+          <t>LSZZ</t>
         </is>
       </c>
       <c r="O26" s="27" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2696,7 +2696,7 @@
       </c>
       <c r="B27" s="27" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>24</t>
         </is>
       </c>
       <c r="C27" s="27" t="n">
@@ -2707,12 +2707,12 @@
       </c>
       <c r="E27" s="27" t="inlineStr">
         <is>
-          <t>1506</t>
+          <t>1411</t>
         </is>
       </c>
       <c r="F27" s="27" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G27" s="27" t="n">
@@ -2725,7 +2725,7 @@
       </c>
       <c r="I27" s="27" t="inlineStr">
         <is>
-          <t>HBWYC</t>
+          <t>HBKLA</t>
         </is>
       </c>
       <c r="J27" s="27" t="inlineStr">
@@ -2744,12 +2744,12 @@
       </c>
       <c r="N27" s="27" t="inlineStr">
         <is>
-          <t>LSZT</t>
+          <t>LSZZ</t>
         </is>
       </c>
       <c r="O27" s="27" t="inlineStr">
         <is>
-          <t>SW</t>
+          <t>SO</t>
         </is>
       </c>
     </row>
@@ -2772,7 +2772,7 @@
       </c>
       <c r="E28" s="27" t="inlineStr">
         <is>
-          <t>0835</t>
+          <t>1436</t>
         </is>
       </c>
       <c r="F28" s="27" t="inlineStr">
@@ -2790,12 +2790,12 @@
       </c>
       <c r="I28" s="27" t="inlineStr">
         <is>
-          <t>HBKFW</t>
+          <t>HBETG</t>
         </is>
       </c>
       <c r="J28" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>06</t>
         </is>
       </c>
       <c r="K28" s="27" t="n">
@@ -2837,12 +2837,12 @@
       </c>
       <c r="E29" s="27" t="inlineStr">
         <is>
-          <t>0835</t>
+          <t>1459</t>
         </is>
       </c>
       <c r="F29" s="27" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G29" s="27" t="n">
@@ -2860,11 +2860,11 @@
       </c>
       <c r="J29" s="27" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>24</t>
         </is>
       </c>
       <c r="K29" s="27" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L29" s="27" t="n">
         <v>0</v>
@@ -2874,12 +2874,12 @@
       </c>
       <c r="N29" s="27" t="inlineStr">
         <is>
-          <t>LSZT</t>
+          <t>LSZZ</t>
         </is>
       </c>
       <c r="O29" s="27" t="inlineStr">
         <is>
-          <t>SW</t>
+          <t>SO</t>
         </is>
       </c>
     </row>
@@ -2902,7 +2902,7 @@
       </c>
       <c r="E30" s="27" t="inlineStr">
         <is>
-          <t>0843</t>
+          <t>1539</t>
         </is>
       </c>
       <c r="F30" s="27" t="inlineStr">
@@ -2920,7 +2920,7 @@
       </c>
       <c r="I30" s="27" t="inlineStr">
         <is>
-          <t>HBKFW</t>
+          <t>HBKLA</t>
         </is>
       </c>
       <c r="J30" s="27" t="inlineStr">
@@ -2939,12 +2939,12 @@
       </c>
       <c r="N30" s="27" t="inlineStr">
         <is>
-          <t>LSZT</t>
+          <t>LSZZ</t>
         </is>
       </c>
       <c r="O30" s="27" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SO</t>
         </is>
       </c>
     </row>
@@ -2967,12 +2967,12 @@
       </c>
       <c r="E31" s="27" t="inlineStr">
         <is>
-          <t>0921</t>
+          <t>1549</t>
         </is>
       </c>
       <c r="F31" s="27" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>V</t>
         </is>
       </c>
       <c r="G31" s="27" t="n">
@@ -2985,7 +2985,7 @@
       </c>
       <c r="I31" s="27" t="inlineStr">
         <is>
-          <t>HBKFW</t>
+          <t>HBETG</t>
         </is>
       </c>
       <c r="J31" s="27" t="inlineStr">
@@ -2994,7 +2994,7 @@
         </is>
       </c>
       <c r="K31" s="27" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L31" s="27" t="n">
         <v>0</v>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="O31" s="27" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -3032,7 +3032,7 @@
       </c>
       <c r="E32" s="27" t="inlineStr">
         <is>
-          <t>0924</t>
+          <t>1557</t>
         </is>
       </c>
       <c r="F32" s="27" t="inlineStr">
@@ -3050,12 +3050,12 @@
       </c>
       <c r="I32" s="27" t="inlineStr">
         <is>
-          <t>HBKFW</t>
+          <t>HBETG</t>
         </is>
       </c>
       <c r="J32" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>06</t>
         </is>
       </c>
       <c r="K32" s="27" t="n">
@@ -3086,7 +3086,7 @@
       </c>
       <c r="B33" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C33" s="27" t="n">
@@ -3102,7 +3102,7 @@
       </c>
       <c r="F33" s="27" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G33" s="27" t="n">
@@ -3115,16 +3115,16 @@
       </c>
       <c r="I33" s="27" t="inlineStr">
         <is>
-          <t>HBYVC</t>
+          <t>HBKLA</t>
         </is>
       </c>
       <c r="J33" s="27" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>24</t>
         </is>
       </c>
       <c r="K33" s="27" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L33" s="27" t="n">
         <v>0</v>
@@ -3134,12 +3134,12 @@
       </c>
       <c r="N33" s="27" t="inlineStr">
         <is>
-          <t>LSZT</t>
+          <t>LSZZ</t>
         </is>
       </c>
       <c r="O33" s="27" t="inlineStr">
         <is>
-          <t>SW</t>
+          <t>SO</t>
         </is>
       </c>
     </row>
@@ -3151,7 +3151,7 @@
       </c>
       <c r="B34" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C34" s="27" t="n">
@@ -3162,7 +3162,7 @@
       </c>
       <c r="E34" s="27" t="inlineStr">
         <is>
-          <t>1008</t>
+          <t>1034</t>
         </is>
       </c>
       <c r="F34" s="27" t="inlineStr">
@@ -3180,12 +3180,12 @@
       </c>
       <c r="I34" s="27" t="inlineStr">
         <is>
-          <t>HBYVC</t>
+          <t>HBKLR</t>
         </is>
       </c>
       <c r="J34" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>06</t>
         </is>
       </c>
       <c r="K34" s="27" t="n">
@@ -3199,7 +3199,7 @@
       </c>
       <c r="N34" s="27" t="inlineStr">
         <is>
-          <t>LSZZ</t>
+          <t>LSZT</t>
         </is>
       </c>
       <c r="O34" s="27" t="inlineStr">
@@ -3216,7 +3216,7 @@
       </c>
       <c r="B35" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C35" s="27" t="n">
@@ -3227,7 +3227,7 @@
       </c>
       <c r="E35" s="27" t="inlineStr">
         <is>
-          <t>1027</t>
+          <t>1042</t>
         </is>
       </c>
       <c r="F35" s="27" t="inlineStr">
@@ -3245,16 +3245,16 @@
       </c>
       <c r="I35" s="27" t="inlineStr">
         <is>
-          <t>HBKLD</t>
+          <t>HBKLR</t>
         </is>
       </c>
       <c r="J35" s="27" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>24</t>
         </is>
       </c>
       <c r="K35" s="27" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L35" s="27" t="n">
         <v>0</v>
@@ -3269,7 +3269,7 @@
       </c>
       <c r="O35" s="27" t="inlineStr">
         <is>
-          <t>SW</t>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="B36" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C36" s="27" t="n">
@@ -3292,12 +3292,12 @@
       </c>
       <c r="E36" s="27" t="inlineStr">
         <is>
-          <t>1032</t>
+          <t>1050</t>
         </is>
       </c>
       <c r="F36" s="27" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G36" s="27" t="n">
@@ -3310,12 +3310,12 @@
       </c>
       <c r="I36" s="27" t="inlineStr">
         <is>
-          <t>HBKLD</t>
+          <t>HBKLR</t>
         </is>
       </c>
       <c r="J36" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>06</t>
         </is>
       </c>
       <c r="K36" s="27" t="n">
@@ -3346,7 +3346,7 @@
       </c>
       <c r="B37" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C37" s="27" t="n">
@@ -3357,12 +3357,12 @@
       </c>
       <c r="E37" s="27" t="inlineStr">
         <is>
-          <t>1036</t>
+          <t>1235</t>
         </is>
       </c>
       <c r="F37" s="27" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G37" s="27" t="n">
@@ -3375,12 +3375,12 @@
       </c>
       <c r="I37" s="27" t="inlineStr">
         <is>
-          <t>HBKLD</t>
+          <t>HBKLR</t>
         </is>
       </c>
       <c r="J37" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>06</t>
         </is>
       </c>
       <c r="K37" s="27" t="n">
@@ -3411,7 +3411,7 @@
       </c>
       <c r="B38" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C38" s="27" t="n">
@@ -3422,7 +3422,7 @@
       </c>
       <c r="E38" s="27" t="inlineStr">
         <is>
-          <t>1044</t>
+          <t>1334</t>
         </is>
       </c>
       <c r="F38" s="27" t="inlineStr">
@@ -3440,12 +3440,12 @@
       </c>
       <c r="I38" s="27" t="inlineStr">
         <is>
-          <t>HBYVC</t>
+          <t>HBKLR</t>
         </is>
       </c>
       <c r="J38" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>06</t>
         </is>
       </c>
       <c r="K38" s="27" t="n">
@@ -3459,12 +3459,12 @@
       </c>
       <c r="N38" s="27" t="inlineStr">
         <is>
-          <t>LSZZ</t>
+          <t>LSZT</t>
         </is>
       </c>
       <c r="O38" s="27" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SO</t>
         </is>
       </c>
     </row>
@@ -3476,7 +3476,7 @@
       </c>
       <c r="B39" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C39" s="27" t="n">
@@ -3487,12 +3487,12 @@
       </c>
       <c r="E39" s="27" t="inlineStr">
         <is>
-          <t>1055</t>
+          <t>1412</t>
         </is>
       </c>
       <c r="F39" s="27" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G39" s="27" t="n">
@@ -3505,7 +3505,7 @@
       </c>
       <c r="I39" s="27" t="inlineStr">
         <is>
-          <t>HBKLD</t>
+          <t>HBKLR</t>
         </is>
       </c>
       <c r="J39" s="27" t="inlineStr">
@@ -3514,7 +3514,7 @@
         </is>
       </c>
       <c r="K39" s="27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L39" s="27" t="n">
         <v>0</v>
@@ -3541,7 +3541,7 @@
       </c>
       <c r="B40" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C40" s="27" t="n">
@@ -3552,7 +3552,7 @@
       </c>
       <c r="E40" s="27" t="inlineStr">
         <is>
-          <t>1059</t>
+          <t>1419</t>
         </is>
       </c>
       <c r="F40" s="27" t="inlineStr">
@@ -3570,7 +3570,7 @@
       </c>
       <c r="I40" s="27" t="inlineStr">
         <is>
-          <t>HBKLD</t>
+          <t>HBKLA</t>
         </is>
       </c>
       <c r="J40" s="27" t="inlineStr">
@@ -3594,7 +3594,7 @@
       </c>
       <c r="O40" s="27" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SO</t>
         </is>
       </c>
     </row>
@@ -3617,12 +3617,12 @@
       </c>
       <c r="E41" s="27" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>1443</t>
         </is>
       </c>
       <c r="F41" s="27" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G41" s="27" t="n">
@@ -3635,12 +3635,12 @@
       </c>
       <c r="I41" s="27" t="inlineStr">
         <is>
-          <t>HBKLA</t>
+          <t>HBKLR</t>
         </is>
       </c>
       <c r="J41" s="27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>06</t>
         </is>
       </c>
       <c r="K41" s="27" t="n">
@@ -3659,7 +3659,7 @@
       </c>
       <c r="O41" s="27" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>NW</t>
         </is>
       </c>
     </row>
@@ -3682,12 +3682,12 @@
       </c>
       <c r="E42" s="27" t="inlineStr">
         <is>
-          <t>1005</t>
+          <t>1500</t>
         </is>
       </c>
       <c r="F42" s="27" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G42" s="27" t="n">
@@ -3700,7 +3700,7 @@
       </c>
       <c r="I42" s="27" t="inlineStr">
         <is>
-          <t>HBKLA</t>
+          <t>HBKLR</t>
         </is>
       </c>
       <c r="J42" s="27" t="inlineStr">
@@ -3747,12 +3747,12 @@
       </c>
       <c r="E43" s="27" t="inlineStr">
         <is>
-          <t>1022</t>
+          <t>1532</t>
         </is>
       </c>
       <c r="F43" s="27" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G43" s="27" t="n">
@@ -3774,7 +3774,7 @@
         </is>
       </c>
       <c r="K43" s="27" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="L43" s="27" t="n">
         <v>0</v>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="O43" s="27" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SO</t>
         </is>
       </c>
     </row>
@@ -3812,12 +3812,12 @@
       </c>
       <c r="E44" s="27" t="inlineStr">
         <is>
-          <t>1034</t>
+          <t>1535</t>
         </is>
       </c>
       <c r="F44" s="27" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G44" s="27" t="n">
@@ -3830,12 +3830,12 @@
       </c>
       <c r="I44" s="27" t="inlineStr">
         <is>
-          <t>HBKLR</t>
+          <t>HBWYC</t>
         </is>
       </c>
       <c r="J44" s="27" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>24</t>
         </is>
       </c>
       <c r="K44" s="27" t="n">
@@ -3849,12 +3849,12 @@
       </c>
       <c r="N44" s="27" t="inlineStr">
         <is>
-          <t>LSZT</t>
+          <t>LSZZ</t>
         </is>
       </c>
       <c r="O44" s="27" t="inlineStr">
         <is>
-          <t>SW</t>
+          <t>NW</t>
         </is>
       </c>
     </row>
@@ -3866,7 +3866,7 @@
       </c>
       <c r="B45" s="27" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>26</t>
         </is>
       </c>
       <c r="C45" s="27" t="n">
@@ -3877,12 +3877,12 @@
       </c>
       <c r="E45" s="27" t="inlineStr">
         <is>
-          <t>1050</t>
+          <t>1301</t>
         </is>
       </c>
       <c r="F45" s="27" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G45" s="27" t="n">
@@ -3895,12 +3895,12 @@
       </c>
       <c r="I45" s="27" t="inlineStr">
         <is>
-          <t>HBKLR</t>
+          <t>HBETG</t>
         </is>
       </c>
       <c r="J45" s="27" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>24</t>
         </is>
       </c>
       <c r="K45" s="27" t="n">
@@ -3914,12 +3914,12 @@
       </c>
       <c r="N45" s="27" t="inlineStr">
         <is>
-          <t>LSZT</t>
+          <t>LSZZ</t>
         </is>
       </c>
       <c r="O45" s="27" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>SW</t>
         </is>
       </c>
     </row>
@@ -3931,7 +3931,7 @@
       </c>
       <c r="B46" s="27" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>26</t>
         </is>
       </c>
       <c r="C46" s="27" t="n">
@@ -3942,12 +3942,12 @@
       </c>
       <c r="E46" s="27" t="inlineStr">
         <is>
-          <t>1222</t>
+          <t>1519</t>
         </is>
       </c>
       <c r="F46" s="27" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G46" s="27" t="n">
@@ -3960,16 +3960,16 @@
       </c>
       <c r="I46" s="27" t="inlineStr">
         <is>
-          <t>HBKLR</t>
+          <t>HBETG</t>
         </is>
       </c>
       <c r="J46" s="27" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>24</t>
         </is>
       </c>
       <c r="K46" s="27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L46" s="27" t="n">
         <v>0</v>
@@ -3979,1120 +3979,30 @@
       </c>
       <c r="N46" s="27" t="inlineStr">
         <is>
-          <t>LSZT</t>
+          <t>LSZZ</t>
         </is>
       </c>
       <c r="O46" s="27" t="inlineStr">
         <is>
-          <t>SW</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="B47" s="27" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="C47" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D47" s="27" t="n">
-        <v>2025</v>
-      </c>
-      <c r="E47" s="27" t="inlineStr">
-        <is>
-          <t>1235</t>
-        </is>
-      </c>
-      <c r="F47" s="27" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="G47" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="H47" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I47" s="27" t="inlineStr">
-        <is>
-          <t>HBKLR</t>
-        </is>
-      </c>
-      <c r="J47" s="27" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="K47" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L47" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M47" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N47" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="O47" s="27" t="inlineStr">
-        <is>
           <t>SO</t>
         </is>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="B48" s="27" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="C48" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D48" s="27" t="n">
-        <v>2025</v>
-      </c>
-      <c r="E48" s="27" t="inlineStr">
-        <is>
-          <t>1239</t>
-        </is>
-      </c>
-      <c r="F48" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="G48" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="H48" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I48" s="27" t="inlineStr">
-        <is>
-          <t>HBKLR</t>
-        </is>
-      </c>
-      <c r="J48" s="27" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="K48" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L48" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M48" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N48" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="O48" s="27" t="inlineStr">
-        <is>
-          <t>SO</t>
-        </is>
-      </c>
-    </row>
-    <row r="49" s="20">
-      <c r="A49" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="B49" s="27" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="C49" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D49" s="27" t="n">
-        <v>2025</v>
-      </c>
-      <c r="E49" s="27" t="inlineStr">
-        <is>
-          <t>1304</t>
-        </is>
-      </c>
-      <c r="F49" s="27" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="G49" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="H49" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I49" s="27" t="inlineStr">
-        <is>
-          <t>HBWYC</t>
-        </is>
-      </c>
-      <c r="J49" s="27" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
-      </c>
-      <c r="K49" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L49" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M49" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N49" s="27" t="inlineStr">
-        <is>
-          <t>LSZZ</t>
-        </is>
-      </c>
-      <c r="O49" s="27" t="inlineStr">
-        <is>
-          <t>SW</t>
-        </is>
-      </c>
-    </row>
-    <row r="50" s="20">
-      <c r="A50" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="B50" s="27" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="C50" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D50" s="27" t="n">
-        <v>2025</v>
-      </c>
-      <c r="E50" s="27" t="inlineStr">
-        <is>
-          <t>1330</t>
-        </is>
-      </c>
-      <c r="F50" s="27" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="G50" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="H50" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I50" s="27" t="inlineStr">
-        <is>
-          <t>HBKLR</t>
-        </is>
-      </c>
-      <c r="J50" s="27" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
-      </c>
-      <c r="K50" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L50" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M50" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N50" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="O50" s="27" t="inlineStr">
-        <is>
-          <t>SO</t>
-        </is>
-      </c>
-    </row>
-    <row r="51" s="20">
-      <c r="A51" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="B51" s="27" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="C51" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D51" s="27" t="n">
-        <v>2025</v>
-      </c>
-      <c r="E51" s="27" t="inlineStr">
-        <is>
-          <t>1334</t>
-        </is>
-      </c>
-      <c r="F51" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="G51" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="H51" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I51" s="27" t="inlineStr">
-        <is>
-          <t>HBKLR</t>
-        </is>
-      </c>
-      <c r="J51" s="27" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
-      </c>
-      <c r="K51" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L51" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M51" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N51" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="O51" s="27" t="inlineStr">
-        <is>
-          <t>SO</t>
-        </is>
-      </c>
-    </row>
-    <row r="52" s="20">
-      <c r="A52" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="B52" s="27" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="C52" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D52" s="27" t="n">
-        <v>2025</v>
-      </c>
-      <c r="E52" s="27" t="inlineStr">
-        <is>
-          <t>1400</t>
-        </is>
-      </c>
-      <c r="F52" s="27" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="G52" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="H52" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I52" s="27" t="inlineStr">
-        <is>
-          <t>HBKLR</t>
-        </is>
-      </c>
-      <c r="J52" s="27" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="K52" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="L52" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M52" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N52" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="O52" s="27" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="53" s="20">
-      <c r="A53" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="B53" s="27" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="C53" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D53" s="27" t="n">
-        <v>2025</v>
-      </c>
-      <c r="E53" s="27" t="inlineStr">
-        <is>
-          <t>1412</t>
-        </is>
-      </c>
-      <c r="F53" s="27" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="G53" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="H53" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I53" s="27" t="inlineStr">
-        <is>
-          <t>HBKLR</t>
-        </is>
-      </c>
-      <c r="J53" s="27" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
-      </c>
-      <c r="K53" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L53" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M53" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N53" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="O53" s="27" t="inlineStr">
-        <is>
-          <t>SW</t>
-        </is>
-      </c>
-    </row>
-    <row r="54" ht="14.25" customHeight="1" s="20">
-      <c r="A54" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="B54" s="27" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="C54" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D54" s="27" t="n">
-        <v>2025</v>
-      </c>
-      <c r="E54" s="27" t="inlineStr">
-        <is>
-          <t>1413</t>
-        </is>
-      </c>
-      <c r="F54" s="27" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="G54" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="H54" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I54" s="27" t="inlineStr">
-        <is>
-          <t>HBKLA</t>
-        </is>
-      </c>
-      <c r="J54" s="27" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
-      </c>
-      <c r="K54" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L54" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M54" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N54" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="O54" s="27" t="inlineStr">
-        <is>
-          <t>SO</t>
-        </is>
-      </c>
-    </row>
-    <row r="55" s="20">
-      <c r="A55" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="B55" s="27" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="C55" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D55" s="27" t="n">
-        <v>2025</v>
-      </c>
-      <c r="E55" s="27" t="inlineStr">
-        <is>
-          <t>1419</t>
-        </is>
-      </c>
-      <c r="F55" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="G55" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="H55" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I55" s="27" t="inlineStr">
-        <is>
-          <t>HBKLA</t>
-        </is>
-      </c>
-      <c r="J55" s="27" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="K55" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L55" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M55" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N55" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="O55" s="27" t="inlineStr">
-        <is>
-          <t>SO</t>
-        </is>
-      </c>
-    </row>
-    <row r="56" s="20">
-      <c r="A56" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="B56" s="27" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="C56" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D56" s="27" t="n">
-        <v>2025</v>
-      </c>
-      <c r="E56" s="27" t="inlineStr">
-        <is>
-          <t>1504</t>
-        </is>
-      </c>
-      <c r="F56" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="G56" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="H56" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I56" s="27" t="inlineStr">
-        <is>
-          <t>HBKLR</t>
-        </is>
-      </c>
-      <c r="J56" s="27" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="K56" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L56" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M56" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N56" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="O56" s="27" t="inlineStr">
-        <is>
-          <t>NW</t>
-        </is>
-      </c>
-    </row>
-    <row r="57" s="20">
-      <c r="A57" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="B57" s="27" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="C57" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D57" s="27" t="n">
-        <v>2025</v>
-      </c>
-      <c r="E57" s="27" t="inlineStr">
-        <is>
-          <t>1526</t>
-        </is>
-      </c>
-      <c r="F57" s="27" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="G57" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="H57" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I57" s="27" t="inlineStr">
-        <is>
-          <t>HBKLR</t>
-        </is>
-      </c>
-      <c r="J57" s="27" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
-      </c>
-      <c r="K57" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L57" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M57" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N57" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="O57" s="27" t="inlineStr">
-        <is>
-          <t>SO</t>
-        </is>
-      </c>
-    </row>
-    <row r="58" s="20">
-      <c r="A58" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="B58" s="27" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="C58" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D58" s="27" t="n">
-        <v>2025</v>
-      </c>
-      <c r="E58" s="27" t="inlineStr">
-        <is>
-          <t>1532</t>
-        </is>
-      </c>
-      <c r="F58" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="G58" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="H58" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I58" s="27" t="inlineStr">
-        <is>
-          <t>HBKLR</t>
-        </is>
-      </c>
-      <c r="J58" s="27" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="K58" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L58" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M58" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N58" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="O58" s="27" t="inlineStr">
-        <is>
-          <t>SO</t>
-        </is>
-      </c>
-    </row>
-    <row r="59" s="20">
-      <c r="A59" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="B59" s="27" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="C59" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D59" s="27" t="n">
-        <v>2025</v>
-      </c>
-      <c r="E59" s="27" t="inlineStr">
-        <is>
-          <t>1535</t>
-        </is>
-      </c>
-      <c r="F59" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="G59" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="H59" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I59" s="27" t="inlineStr">
-        <is>
-          <t>HBWYC</t>
-        </is>
-      </c>
-      <c r="J59" s="27" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="K59" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L59" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M59" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N59" s="27" t="inlineStr">
-        <is>
-          <t>LSZZ</t>
-        </is>
-      </c>
-      <c r="O59" s="27" t="inlineStr">
-        <is>
-          <t>NW</t>
-        </is>
-      </c>
-    </row>
-    <row r="60" s="20">
-      <c r="A60" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="B60" s="27" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="C60" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D60" s="27" t="n">
-        <v>2025</v>
-      </c>
-      <c r="E60" s="27" t="inlineStr">
-        <is>
-          <t>1243</t>
-        </is>
-      </c>
-      <c r="F60" s="27" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="G60" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="H60" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I60" s="27" t="inlineStr">
-        <is>
-          <t>HBETG</t>
-        </is>
-      </c>
-      <c r="J60" s="27" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
-      </c>
-      <c r="K60" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="L60" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M60" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N60" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="O60" s="27" t="inlineStr">
-        <is>
-          <t>SW</t>
-        </is>
-      </c>
-    </row>
-    <row r="61" s="20">
-      <c r="A61" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="B61" s="27" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="C61" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D61" s="27" t="n">
-        <v>2025</v>
-      </c>
-      <c r="E61" s="27" t="inlineStr">
-        <is>
-          <t>1301</t>
-        </is>
-      </c>
-      <c r="F61" s="27" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="G61" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="H61" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I61" s="27" t="inlineStr">
-        <is>
-          <t>HBETG</t>
-        </is>
-      </c>
-      <c r="J61" s="27" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="K61" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L61" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M61" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N61" s="27" t="inlineStr">
-        <is>
-          <t>LSZZ</t>
-        </is>
-      </c>
-      <c r="O61" s="27" t="inlineStr">
-        <is>
-          <t>SW</t>
-        </is>
-      </c>
-    </row>
-    <row r="62" s="20">
-      <c r="A62" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="B62" s="27" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="C62" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D62" s="27" t="n">
-        <v>2025</v>
-      </c>
-      <c r="E62" s="27" t="inlineStr">
-        <is>
-          <t>1514</t>
-        </is>
-      </c>
-      <c r="F62" s="27" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="G62" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="H62" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I62" s="27" t="inlineStr">
-        <is>
-          <t>HBETG</t>
-        </is>
-      </c>
-      <c r="J62" s="27" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
-      </c>
-      <c r="K62" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L62" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M62" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N62" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="O62" s="27" t="inlineStr">
-        <is>
-          <t>SO</t>
-        </is>
-      </c>
-    </row>
-    <row r="63" s="20">
-      <c r="A63" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="B63" s="27" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="C63" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D63" s="27" t="n">
-        <v>2025</v>
-      </c>
-      <c r="E63" s="27" t="inlineStr">
-        <is>
-          <t>1519</t>
-        </is>
-      </c>
-      <c r="F63" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="G63" s="27" t="n">
-        <v>4</v>
-      </c>
-      <c r="H63" s="27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I63" s="27" t="inlineStr">
-        <is>
-          <t>HBETG</t>
-        </is>
-      </c>
-      <c r="J63" s="27" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="K63" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L63" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M63" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N63" s="27" t="inlineStr">
-        <is>
-          <t>LSZT</t>
-        </is>
-      </c>
-      <c r="O63" s="27" t="inlineStr">
-        <is>
-          <t>SO</t>
-        </is>
-      </c>
-    </row>
+    <row r="49" s="20"/>
+    <row r="50" s="20"/>
+    <row r="51" s="20"/>
+    <row r="52" s="20"/>
+    <row r="53" s="20"/>
+    <row r="54" ht="14.25" customHeight="1" s="20"/>
+    <row r="55" s="20"/>
+    <row r="56" s="20"/>
+    <row r="57" s="20"/>
+    <row r="58" s="20"/>
+    <row r="59" s="20"/>
+    <row r="60" s="20"/>
+    <row r="61" s="20"/>
+    <row r="62" s="20"/>
+    <row r="63" s="20"/>
   </sheetData>
   <pageMargins left="0.7874015748031497" right="0.7874015748031497" top="0.984251968503937" bottom="0.984251968503937" header="0.5118110236220472" footer="0.5118110236220472"/>
   <pageSetup orientation="landscape" paperSize="8" scale="79"/>

</xml_diff>